<commit_message>
a little new data
</commit_message>
<xml_diff>
--- a/different methods/experiment_2018_9_18_15_47_45.xlsx
+++ b/different methods/experiment_2018_9_18_15_47_45.xlsx
@@ -30282,7 +30282,7 @@
   <dimension ref="A1:AY100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AH17" workbookViewId="0">
-      <selection activeCell="AY37" sqref="AY37"/>
+      <selection activeCell="AY43" sqref="AY43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36173,6 +36173,9 @@
       <c r="AX38">
         <v>0.55400000000000005</v>
       </c>
+      <c r="AY38">
+        <v>0.58599999999999997</v>
+      </c>
     </row>
     <row r="39" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A39">
@@ -36325,6 +36328,9 @@
       <c r="AX39">
         <v>0.52300000000000002</v>
       </c>
+      <c r="AY39">
+        <v>0.55800000000000005</v>
+      </c>
     </row>
     <row r="40" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A40">
@@ -36477,6 +36483,9 @@
       <c r="AX40">
         <v>0.56100000000000005</v>
       </c>
+      <c r="AY40">
+        <v>0.55200000000000005</v>
+      </c>
     </row>
     <row r="41" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A41">
@@ -36629,6 +36638,9 @@
       <c r="AX41">
         <v>0.53500000000000003</v>
       </c>
+      <c r="AY41">
+        <v>0.52100000000000002</v>
+      </c>
     </row>
     <row r="42" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A42">
@@ -36781,6 +36793,9 @@
       <c r="AX42">
         <v>0.54900000000000004</v>
       </c>
+      <c r="AY42">
+        <v>0.56000000000000005</v>
+      </c>
     </row>
     <row r="43" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A43">
@@ -36932,6 +36947,9 @@
       </c>
       <c r="AX43">
         <v>0.53800000000000003</v>
+      </c>
+      <c r="AY43">
+        <v>0.57899999999999996</v>
       </c>
     </row>
     <row r="44" spans="1:51" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
a little little more data
</commit_message>
<xml_diff>
--- a/different methods/experiment_2018_9_18_15_47_45.xlsx
+++ b/different methods/experiment_2018_9_18_15_47_45.xlsx
@@ -30282,7 +30282,7 @@
   <dimension ref="A1:AY100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AH17" workbookViewId="0">
-      <selection activeCell="AY43" sqref="AY43"/>
+      <selection activeCell="AY45" sqref="AY45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37103,6 +37103,9 @@
       <c r="AX44">
         <v>0.55300000000000005</v>
       </c>
+      <c r="AY44">
+        <v>0.57699999999999996</v>
+      </c>
     </row>
     <row r="45" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A45">
@@ -37254,6 +37257,9 @@
       </c>
       <c r="AX45">
         <v>0.56599999999999995</v>
+      </c>
+      <c r="AY45">
+        <v>0.55700000000000005</v>
       </c>
     </row>
     <row r="46" spans="1:51" x14ac:dyDescent="0.25">

</xml_diff>